<commit_message>
11주차 frontend 로그인, 게시판 api fetch 작업1
</commit_message>
<xml_diff>
--- a/project1_GameRoom/Project/GameRoom-변수설정.xlsx
+++ b/project1_GameRoom/Project/GameRoom-변수설정.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Atom\GameRoom\project1_GameRoom\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9884D859-D96E-4A30-B85F-FE56BAE7E43D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA837EFE-1F73-4555-8281-0A0F212AD7B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -92,12 +92,6 @@
   </si>
   <si>
     <t>/api/board</t>
-  </si>
-  <si>
-    <t>{
-   title: "게시글1",
-   content: "안녕하세요"
-}</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -927,6 +921,55 @@
     </r>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
+  <si>
+    <r>
+      <t>{
+   title: "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>게시글</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1",
+   content: "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>안녕하세요</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"
+}</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -1321,8 +1364,8 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1390,7 +1433,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>11</v>
@@ -1460,7 +1503,7 @@
         <v>10</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>16</v>
@@ -1488,19 +1531,19 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1">
       <c r="A5" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>48</v>
-      </c>
       <c r="C5" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>17</v>
@@ -1530,8 +1573,8 @@
       <c r="A6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>14</v>
+      <c r="B6" s="14" t="s">
+        <v>51</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>19</v>
@@ -1539,7 +1582,7 @@
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="8"/>
@@ -1562,7 +1605,7 @@
       <c r="Y6" s="10"/>
       <c r="Z6" s="10"/>
     </row>
-    <row r="7" spans="1:26" ht="12.75">
+    <row r="7" spans="1:26" ht="52.5">
       <c r="A7" s="7" t="s">
         <v>20</v>
       </c>
@@ -1575,11 +1618,11 @@
       <c r="D7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>22</v>
+      <c r="E7" s="18" t="s">
+        <v>68</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="8"/>
@@ -1604,22 +1647,22 @@
     </row>
     <row r="8" spans="1:26" ht="409.5">
       <c r="A8" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="E8" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>27</v>
-      </c>
       <c r="F8" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G8" s="9"/>
       <c r="H8" s="8"/>
@@ -1644,25 +1687,25 @@
     </row>
     <row r="9" spans="1:26" ht="12.75">
       <c r="A9" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="C9" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="D9" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="E9" s="7" t="s">
         <v>31</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>32</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>11</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H9" s="11"/>
       <c r="I9" s="7"/>
@@ -1686,22 +1729,22 @@
     </row>
     <row r="10" spans="1:26" ht="12.75">
       <c r="A10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>35</v>
-      </c>
       <c r="C10" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D10" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>27</v>
-      </c>
       <c r="F10" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G10" s="9"/>
       <c r="H10" s="8"/>
@@ -1726,22 +1769,22 @@
     </row>
     <row r="11" spans="1:26" ht="12.75">
       <c r="A11" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
@@ -1766,22 +1809,22 @@
     </row>
     <row r="12" spans="1:26" ht="12.75">
       <c r="A12" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
@@ -1806,22 +1849,22 @@
     </row>
     <row r="13" spans="1:26" ht="12.75">
       <c r="A13" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="7" t="s">
+      <c r="F13" s="7" t="s">
         <v>44</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>45</v>
       </c>
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
@@ -1846,22 +1889,22 @@
     </row>
     <row r="14" spans="1:26" ht="409.5">
       <c r="A14" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="D14" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" s="14" t="s">
+      <c r="E14" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E14" s="14" t="s">
-        <v>54</v>
-      </c>
       <c r="F14" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
@@ -1886,18 +1929,18 @@
     </row>
     <row r="15" spans="1:26" ht="38.25">
       <c r="A15" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
       <c r="F15" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
@@ -1922,22 +1965,22 @@
     </row>
     <row r="16" spans="1:26" ht="409.5">
       <c r="A16" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="C16" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="D16" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="E16" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="F16" s="18" t="s">
         <v>65</v>
-      </c>
-      <c r="F16" s="18" t="s">
-        <v>66</v>
       </c>
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>

</xml_diff>